<commit_message>
made changes to script
</commit_message>
<xml_diff>
--- a/2015_BombSurv_Plants/2015_BombSurv_PlantDensity.xlsx
+++ b/2015_BombSurv_Plants/2015_BombSurv_PlantDensity.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipburnham/Desktop/RScripts/2015_BombSurv_Plants/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipburnham/Documents/GitHub/AlgerProjects/2015_BombSurv_Plants/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -742,8 +742,8 @@
   <dimension ref="A1:BQ999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BP2" sqref="BP2"/>
+      <pane xSplit="1" topLeftCell="BA1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BC12" sqref="BC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>